<commit_message>
Renaming the survey response file
</commit_message>
<xml_diff>
--- a/SoftwareEngineeringSurveyResponses.xlsx
+++ b/SoftwareEngineeringSurveyResponses.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="Calc"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookProtection/>
+  <bookViews>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="0"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Form Responses 1" sheetId="1" r:id="rId3"/>
+    <sheet name="Form Responses 1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="Unspecified"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="101">
-  <si>
-    <t>Timestamp</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="100">
   <si>
     <t>Are you satisfied with default text size and image position or you have to make some adjustments?</t>
   </si>
@@ -25,7 +31,7 @@
     <t>Does frequent scrolling gives your eyes strain?</t>
   </si>
   <si>
-    <t xml:space="preserve">What type of reading issue you encountered while reading exercise? </t>
+    <t>What type of reading issue you encountered while reading exercise? </t>
   </si>
   <si>
     <t>Do you have any suggestion to improve reading quality of webpages?</t>
@@ -127,7 +133,7 @@
     <t>I had to observe the image properly so that I don't have to scroll to it again and again. But it did interrupt my reading twice.</t>
   </si>
   <si>
-    <t xml:space="preserve">I am used to reading e-books, papers and web articles online. I am used to such kinds of scrolling. So don't really feel the strain, but of course, reducing the scrolling would make reading activity easy. </t>
+    <t>I am used to reading e-books, papers and web articles online. I am used to such kinds of scrolling. So don't really feel the strain, but of course, reducing the scrolling would make reading activity easy. </t>
   </si>
   <si>
     <t>Image was not correctly positioned on the web page along with the text.</t>
@@ -213,7 +219,7 @@
     <t>Yes it is very straining for eyes.</t>
   </si>
   <si>
-    <t xml:space="preserve">Every time I had to see an image, the page was required to be scrolled. </t>
+    <t>Every time I had to see an image, the page was required to be scrolled. </t>
   </si>
   <si>
     <t>The image can move along with the text</t>
@@ -252,7 +258,7 @@
     <t>I have to zoom in sometimes</t>
   </si>
   <si>
-    <t xml:space="preserve">some articles contains other components which need to be refereed. I have to go there to see them </t>
+    <t>some articles contains other components which need to be refereed. I have to go there to see them </t>
   </si>
   <si>
     <t>in very long article it does</t>
@@ -321,493 +327,492 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="m/d/yyyy h:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="5">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
-    <font/>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border>
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+  <cellStyleXfs count="20">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+  <cellStyles count="6">
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
-  <dxfs count="0"/>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/worksheetdrawing.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
-</file>
-
-<file path=xl/worksheets/sheet.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="6" width="21.57"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="40.4234693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="43.0714285714286"/>
+    <col collapsed="false" hidden="false" max="5" min="3" style="0" width="21.3265306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="14.1734693877551"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="s">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1">
-        <v>42400.000689259265</v>
-      </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="2" t="s">
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1">
-        <v>42400.00174083334</v>
-      </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="2" t="s">
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1">
-        <v>42400.004241041664</v>
-      </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="2" t="s">
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1">
-        <v>42400.00611567129</v>
-      </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F5" s="2" t="s">
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1">
-        <v>42400.0175725</v>
-      </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="F6" s="2" t="s">
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1">
-        <v>42400.03006263889</v>
-      </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="F7" s="2" t="s">
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1">
-        <v>42400.04057783565</v>
-      </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E8" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F8" s="2" t="s">
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1">
-        <v>42400.054715543985</v>
-      </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="2">
-        <v>2.0</v>
-      </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E9" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F9" s="2" t="s">
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="1">
-        <v>42400.05717719907</v>
-      </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E10" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="F10" s="2" t="s">
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="1">
-        <v>42400.07073119213</v>
-      </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E11" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="F11" s="2" t="s">
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="1">
-        <v>42400.071974942126</v>
-      </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D12" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="E12" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="F12" s="2" t="s">
+    </row>
+    <row r="13" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="1">
-        <v>42400.076146990745</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>41</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="F13" s="2" t="s">
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="1">
-        <v>42400.07640074074</v>
-      </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D14" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="E14" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="F14" s="2" t="s">
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="1">
-        <v>42400.085683136575</v>
-      </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D15" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="E15" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="F15" s="2" t="s">
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="1">
-        <v>42400.490998368055</v>
-      </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D16" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="E16" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="F16" s="2" t="s">
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="1">
-        <v>42400.492803553236</v>
-      </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="D17" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="E17" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="F17" s="2" t="s">
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="1">
-        <v>42400.495650428245</v>
-      </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="D18" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E18" s="2" t="s">
+      <c r="E18" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="F18" s="2" t="s">
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="1">
-        <v>42400.497202557875</v>
-      </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C19" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="D19" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="E19" s="2" t="s">
+      <c r="E19" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="F19" s="2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="1">
-        <v>42400.49923383102</v>
-      </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C20" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="D20" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="E20" s="2" t="s">
+      <c r="E20" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="F20" s="2" t="s">
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="1">
-        <v>42400.50129114583</v>
-      </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C21" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="D21" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="E21" s="2" t="s">
+      <c r="E21" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="F21" s="2" t="s">
-        <v>100</v>
-      </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>